<commit_message>
UI Fixes and some backend fix fo import
</commit_message>
<xml_diff>
--- a/EmployeeDetails.xlsx
+++ b/EmployeeDetails.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShubhamR\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shubham_Workplace\OfficeManagerCommunity\OfficeManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E0DEA7-1352-44C2-9D20-B447B8206438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22951E7F-EA3E-4A13-A324-B4173C39041C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jul 2022" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="242">
   <si>
     <t>Atharva System</t>
   </si>
@@ -752,6 +752,12 @@
   </si>
   <si>
     <t>This report is generated by Keka HR and Payroll Software</t>
+  </si>
+  <si>
+    <t>Test Import</t>
+  </si>
+  <si>
+    <t>abc</t>
   </si>
 </sst>
 </file>
@@ -1131,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3005,6 +3011,26 @@
         <v>36910</v>
       </c>
     </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>189</v>
+      </c>
+      <c r="B95" t="s">
+        <v>240</v>
+      </c>
+      <c r="C95" s="4">
+        <v>44753</v>
+      </c>
+      <c r="D95" t="s">
+        <v>241</v>
+      </c>
+      <c r="E95" t="s">
+        <v>241</v>
+      </c>
+      <c r="F95" s="4">
+        <v>35800</v>
+      </c>
+    </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
         <v>238</v>

</xml_diff>

<commit_message>
UI side issues are fixed, And Import employee functionality is all set from frontend and backend both. removed unused uis from frontend import functionality is working fine
</commit_message>
<xml_diff>
--- a/EmployeeDetails.xlsx
+++ b/EmployeeDetails.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShubhamR\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shubham_Workplace\OfficeManagerCommunity\OfficeManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E0DEA7-1352-44C2-9D20-B447B8206438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22951E7F-EA3E-4A13-A324-B4173C39041C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jul 2022" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="242">
   <si>
     <t>Atharva System</t>
   </si>
@@ -752,6 +752,12 @@
   </si>
   <si>
     <t>This report is generated by Keka HR and Payroll Software</t>
+  </si>
+  <si>
+    <t>Test Import</t>
+  </si>
+  <si>
+    <t>abc</t>
   </si>
 </sst>
 </file>
@@ -1131,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3005,6 +3011,26 @@
         <v>36910</v>
       </c>
     </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>189</v>
+      </c>
+      <c r="B95" t="s">
+        <v>240</v>
+      </c>
+      <c r="C95" s="4">
+        <v>44753</v>
+      </c>
+      <c r="D95" t="s">
+        <v>241</v>
+      </c>
+      <c r="E95" t="s">
+        <v>241</v>
+      </c>
+      <c r="F95" s="4">
+        <v>35800</v>
+      </c>
+    </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
         <v>238</v>

</xml_diff>

<commit_message>
UI fixes as dicussed 1. Added title for import preview 2. Showed highlighted data are not going to inserted and save all the valid data only 3. made backgound disable on load time and loader will active and all other will be disabled 4. put prefix for all search or placeholder
5. button aligned to right for import and add
6. added heading of page in header
</commit_message>
<xml_diff>
--- a/EmployeeDetails.xlsx
+++ b/EmployeeDetails.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shubham_Workplace\OfficeManagerCommunity\OfficeManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shubham_Workplace\OfficeManagerCommunity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22951E7F-EA3E-4A13-A324-B4173C39041C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717AD7F3-E738-4D39-9835-9C530FA9B462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jul 2022" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="241">
   <si>
     <t>Atharva System</t>
   </si>
@@ -755,9 +755,6 @@
   </si>
   <si>
     <t>Test Import</t>
-  </si>
-  <si>
-    <t>abc</t>
   </si>
 </sst>
 </file>
@@ -1138,7 +1135,7 @@
   <dimension ref="A1:F97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3022,10 +3019,10 @@
         <v>44753</v>
       </c>
       <c r="D95" t="s">
-        <v>241</v>
+        <v>197</v>
       </c>
       <c r="E95" t="s">
-        <v>241</v>
+        <v>96</v>
       </c>
       <c r="F95" s="4">
         <v>35800</v>

</xml_diff>

<commit_message>
1. Add title for import preview 2.  show highlighted data are not going to inserted and save all the valid data only 3. make backgound disable on load time and loader will active and all other will be disabled put prefix for all search or placeholder
button align to right for import and add
add heading of page in header
</commit_message>
<xml_diff>
--- a/EmployeeDetails.xlsx
+++ b/EmployeeDetails.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shubham_Workplace\OfficeManagerCommunity\OfficeManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shubham_Workplace\OfficeManagerCommunity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22951E7F-EA3E-4A13-A324-B4173C39041C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717AD7F3-E738-4D39-9835-9C530FA9B462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jul 2022" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="241">
   <si>
     <t>Atharva System</t>
   </si>
@@ -755,9 +755,6 @@
   </si>
   <si>
     <t>Test Import</t>
-  </si>
-  <si>
-    <t>abc</t>
   </si>
 </sst>
 </file>
@@ -1138,7 +1135,7 @@
   <dimension ref="A1:F97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3022,10 +3019,10 @@
         <v>44753</v>
       </c>
       <c r="D95" t="s">
-        <v>241</v>
+        <v>197</v>
       </c>
       <c r="E95" t="s">
-        <v>241</v>
+        <v>96</v>
       </c>
       <c r="F95" s="4">
         <v>35800</v>

</xml_diff>

<commit_message>
Code cleanup in progress
</commit_message>
<xml_diff>
--- a/EmployeeDetails.xlsx
+++ b/EmployeeDetails.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shubham_Workplace\OfficeManagerCommunity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717AD7F3-E738-4D39-9835-9C530FA9B462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EAEA58-C986-4C37-B70A-CA921C28D7ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Jul 2022" sheetId="1" r:id="rId1"/>
+    <sheet name="Employees" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -825,8 +825,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>

</xml_diff>

<commit_message>
Code clean up done for unwanted code in api, command and query.
</commit_message>
<xml_diff>
--- a/EmployeeDetails.xlsx
+++ b/EmployeeDetails.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shubham_Workplace\OfficeManagerCommunity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EAEA58-C986-4C37-B70A-CA921C28D7ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717AD7F3-E738-4D39-9835-9C530FA9B462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Employees" sheetId="1" r:id="rId1"/>
+    <sheet name="Jul 2022" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -825,8 +825,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>

</xml_diff>

<commit_message>
Bulk  Employee Import return  more than one data and save bulk employee is now done by efcore
</commit_message>
<xml_diff>
--- a/EmployeeDetails.xlsx
+++ b/EmployeeDetails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shubham_Workplace\OfficeManagerCommunity\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shubham\OfficeManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717AD7F3-E738-4D39-9835-9C530FA9B462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2967F3-67DB-4C71-B74A-AD0FCB1CD5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3696" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jul 2022" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="240">
   <si>
     <t>Atharva System</t>
   </si>
@@ -748,13 +748,10 @@
     <t>Nimay Vijaybhai Panchal</t>
   </si>
   <si>
-    <t>Generated on 02/08/2022</t>
-  </si>
-  <si>
-    <t>This report is generated by Keka HR and Payroll Software</t>
-  </si>
-  <si>
     <t>Test Import</t>
+  </si>
+  <si>
+    <t>Test Karna</t>
   </si>
 </sst>
 </file>
@@ -825,8 +822,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1134,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3013,7 +3010,7 @@
         <v>189</v>
       </c>
       <c r="B95" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C95" s="4">
         <v>44753</v>
@@ -3028,14 +3025,30 @@
         <v>35800</v>
       </c>
     </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>201</v>
+      </c>
+      <c r="B96" t="s">
+        <v>239</v>
+      </c>
+      <c r="C96" s="4">
+        <v>44753</v>
+      </c>
+      <c r="D96" t="s">
+        <v>197</v>
+      </c>
+      <c r="E96" t="s">
+        <v>96</v>
+      </c>
+      <c r="F96" s="4">
+        <v>35800</v>
+      </c>
+    </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" s="6" t="s">
-        <v>238</v>
-      </c>
+      <c r="A97" s="6"/>
       <c r="B97" s="6"/>
-      <c r="C97" s="7" t="s">
-        <v>239</v>
-      </c>
+      <c r="C97" s="7"/>
       <c r="D97" s="6"/>
       <c r="E97" s="6"/>
       <c r="F97" s="7"/>

</xml_diff>